<commit_message>
- Added the ability to read in data about spells and parse them! This means that an individual spell can now have various effects attached to it. - Removed the old symbol info text file. - Updated data collection excell document.
</commit_message>
<xml_diff>
--- a/Alchemy/data/LetterFreq.xlsx
+++ b/Alchemy/data/LetterFreq.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\alchemy\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reverie\Source\Repos\CBREngine\Alchemy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11610" tabRatio="781" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11610" tabRatio="781" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="High Knockback Spells" sheetId="7" r:id="rId6"/>
     <sheet name="High Recoil Spells" sheetId="8" r:id="rId7"/>
     <sheet name="Names to Credit" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="147">
   <si>
     <t>a</t>
   </si>
@@ -374,6 +375,105 @@
   <si>
     <t>quake</t>
   </si>
+  <si>
+    <t>Letter:</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Instance</t>
+  </si>
+  <si>
+    <t>AOE</t>
+  </si>
+  <si>
+    <t>Knockback</t>
+  </si>
+  <si>
+    <t>Recoil</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
 </sst>
 </file>
 
@@ -941,11 +1041,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="38762576"/>
-        <c:axId val="38769648"/>
+        <c:axId val="-911618896"/>
+        <c:axId val="-911623792"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="38769648"/>
+        <c:axId val="-911623792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,12 +1096,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38762576"/>
+        <c:crossAx val="-911618896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="38762576"/>
+        <c:axId val="-911618896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1044,7 +1144,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38769648"/>
+        <c:crossAx val="-911623792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1418,11 +1518,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="2050305616"/>
-        <c:axId val="1953567552"/>
+        <c:axId val="-907826336"/>
+        <c:axId val="-907818176"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="1953567552"/>
+        <c:axId val="-907818176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,12 +1573,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2050305616"/>
+        <c:crossAx val="-907826336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2050305616"/>
+        <c:axId val="-907826336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,7 +1621,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1953567552"/>
+        <c:crossAx val="-907818176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2062,11 +2162,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="2050299632"/>
-        <c:axId val="2050303984"/>
+        <c:axId val="-907829056"/>
+        <c:axId val="-907829600"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="2050303984"/>
+        <c:axId val="-907829600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2117,12 +2217,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2050299632"/>
+        <c:crossAx val="-907829056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2050299632"/>
+        <c:axId val="-907829056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2165,7 +2265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2050303984"/>
+        <c:crossAx val="-907829600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2539,11 +2639,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="2108570784"/>
-        <c:axId val="2050301264"/>
+        <c:axId val="-907827968"/>
+        <c:axId val="-907821984"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="2050301264"/>
+        <c:axId val="-907821984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2594,12 +2694,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108570784"/>
+        <c:crossAx val="-907827968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2108570784"/>
+        <c:axId val="-907827968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2642,7 +2742,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2050301264"/>
+        <c:crossAx val="-907821984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3183,11 +3283,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="1920456640"/>
-        <c:axId val="2108576224"/>
+        <c:axId val="-907820896"/>
+        <c:axId val="-907822528"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="2108576224"/>
+        <c:axId val="-907822528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3238,12 +3338,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1920456640"/>
+        <c:crossAx val="-907820896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1920456640"/>
+        <c:axId val="-907820896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3286,7 +3386,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108576224"/>
+        <c:crossAx val="-907822528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3660,11 +3760,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="42408768"/>
-        <c:axId val="42408224"/>
+        <c:axId val="-907052864"/>
+        <c:axId val="-907055584"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="42408224"/>
+        <c:axId val="-907055584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3715,12 +3815,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42408768"/>
+        <c:crossAx val="-907052864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="42408768"/>
+        <c:axId val="-907052864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3763,7 +3863,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42408224"/>
+        <c:crossAx val="-907055584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4105,11 +4205,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="38764208"/>
-        <c:axId val="38759856"/>
+        <c:axId val="-911618352"/>
+        <c:axId val="-911631952"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="38759856"/>
+        <c:axId val="-911631952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4160,12 +4260,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38764208"/>
+        <c:crossAx val="-911618352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="38764208"/>
+        <c:axId val="-911618352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4208,7 +4308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38759856"/>
+        <c:crossAx val="-911631952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4749,11 +4849,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="38761488"/>
-        <c:axId val="38768016"/>
+        <c:axId val="-911622160"/>
+        <c:axId val="-911631408"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="38768016"/>
+        <c:axId val="-911631408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4804,12 +4904,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38761488"/>
+        <c:crossAx val="-911622160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="38761488"/>
+        <c:axId val="-911622160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4852,7 +4952,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38768016"/>
+        <c:crossAx val="-911631408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5226,11 +5326,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="38764752"/>
-        <c:axId val="38765296"/>
+        <c:axId val="-911625968"/>
+        <c:axId val="-911627600"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="38765296"/>
+        <c:axId val="-911627600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5281,12 +5381,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38764752"/>
+        <c:crossAx val="-911625968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="38764752"/>
+        <c:axId val="-911625968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5329,7 +5429,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38765296"/>
+        <c:crossAx val="-911627600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5870,11 +5970,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="38766928"/>
-        <c:axId val="38765840"/>
+        <c:axId val="-911621072"/>
+        <c:axId val="-911624880"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="38765840"/>
+        <c:axId val="-911624880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5925,12 +6025,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38766928"/>
+        <c:crossAx val="-911621072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="38766928"/>
+        <c:axId val="-911621072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5973,7 +6073,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38765840"/>
+        <c:crossAx val="-911624880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6347,11 +6447,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="38771280"/>
-        <c:axId val="38770192"/>
+        <c:axId val="-907827424"/>
+        <c:axId val="-1140204080"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="38770192"/>
+        <c:axId val="-1140204080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6402,12 +6502,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38771280"/>
+        <c:crossAx val="-907827424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="38771280"/>
+        <c:axId val="-907827424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6450,7 +6550,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38770192"/>
+        <c:crossAx val="-1140204080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6991,11 +7091,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="38773456"/>
-        <c:axId val="38772912"/>
+        <c:axId val="-907816544"/>
+        <c:axId val="-907819264"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="38772912"/>
+        <c:axId val="-907819264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7046,12 +7146,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38773456"/>
+        <c:crossAx val="-907816544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="38773456"/>
+        <c:axId val="-907816544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7094,7 +7194,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38772912"/>
+        <c:crossAx val="-907819264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7468,11 +7568,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="1953568096"/>
-        <c:axId val="1953563744"/>
+        <c:axId val="-907815456"/>
+        <c:axId val="-907824704"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="1953563744"/>
+        <c:axId val="-907824704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7523,12 +7623,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1953568096"/>
+        <c:crossAx val="-907815456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1953568096"/>
+        <c:axId val="-907815456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7571,7 +7671,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1953563744"/>
+        <c:crossAx val="-907824704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8112,11 +8212,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="15"/>
-        <c:axId val="1953561568"/>
-        <c:axId val="1953576800"/>
+        <c:axId val="-907825792"/>
+        <c:axId val="-907817632"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="1953576800"/>
+        <c:axId val="-907817632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8167,12 +8267,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1953561568"/>
+        <c:crossAx val="-907825792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1953561568"/>
+        <c:axId val="-907825792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8215,7 +8315,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1953576800"/>
+        <c:crossAx val="-907817632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17034,7 +17134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -20441,7 +20541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -21184,4 +21284,796 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2">
+        <f>'High Damage Spells'!D1  / 'High Damage Spells'!E1</f>
+        <v>0.76899908360942526</v>
+      </c>
+      <c r="C2">
+        <f>'High Duration Spells'!D1  / 'High Duration Spells'!E1</f>
+        <v>1.1071268213773888</v>
+      </c>
+      <c r="D2">
+        <f>'High Instance Spells'!D1  / 'High Instance Spells'!E1</f>
+        <v>0.62448480003996698</v>
+      </c>
+      <c r="E2">
+        <f>'AOE Spells'!D1  / 'AOE Spells'!E1</f>
+        <v>1.3752698967172305</v>
+      </c>
+      <c r="F2">
+        <f>'High Knockback Spells'!D1  / 'High Knockback Spells'!E1</f>
+        <v>0.90188752174193121</v>
+      </c>
+      <c r="G2">
+        <f>'High Recoil Spells'!D1  / 'High Recoil Spells'!E1</f>
+        <v>0.78604875748149983</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3">
+        <f>'High Damage Spells'!D2  / 'High Damage Spells'!E2</f>
+        <v>2.1082961453318809</v>
+      </c>
+      <c r="C3">
+        <f>'High Duration Spells'!D2  / 'High Duration Spells'!E2</f>
+        <v>1.0117702606994705</v>
+      </c>
+      <c r="D3">
+        <f>'High Instance Spells'!D2  / 'High Instance Spells'!E2</f>
+        <v>1.3696753869332969</v>
+      </c>
+      <c r="E3">
+        <f>'AOE Spells'!D2  / 'AOE Spells'!E2</f>
+        <v>0.75409094336777016</v>
+      </c>
+      <c r="F3">
+        <f>'High Knockback Spells'!D2  / 'High Knockback Spells'!E2</f>
+        <v>0.70646414694454251</v>
+      </c>
+      <c r="G3">
+        <f>'High Recoil Spells'!D2  / 'High Recoil Spells'!E2</f>
+        <v>1.8471768979742629</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <f>'High Damage Spells'!D3  / 'High Damage Spells'!E3</f>
+        <v>0.75332404233681127</v>
+      </c>
+      <c r="C4">
+        <f>'High Duration Spells'!D3  / 'High Duration Spells'!E3</f>
+        <v>1.0845594880879217</v>
+      </c>
+      <c r="D4">
+        <f>'High Instance Spells'!D3  / 'High Instance Spells'!E3</f>
+        <v>1.101159888415798</v>
+      </c>
+      <c r="E4">
+        <f>'AOE Spells'!D3  / 'AOE Spells'!E3</f>
+        <v>1.2125131355589687</v>
+      </c>
+      <c r="F4">
+        <f>'High Knockback Spells'!D3  / 'High Knockback Spells'!E3</f>
+        <v>1.135933358576297</v>
+      </c>
+      <c r="G4">
+        <f>'High Recoil Spells'!D3  / 'High Recoil Spells'!E3</f>
+        <v>0.9900336611444791</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <f>'High Damage Spells'!D4  / 'High Damage Spells'!E4</f>
+        <v>0.61595318755774553</v>
+      </c>
+      <c r="C5">
+        <f>'High Duration Spells'!D4  / 'High Duration Spells'!E4</f>
+        <v>1.0641442506650902</v>
+      </c>
+      <c r="D5">
+        <f>'High Instance Spells'!D4  / 'High Instance Spells'!E4</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>'AOE Spells'!D4  / 'AOE Spells'!E4</f>
+        <v>0.52875082617316593</v>
+      </c>
+      <c r="F5">
+        <f>'High Knockback Spells'!D4  / 'High Knockback Spells'!E4</f>
+        <v>1.2383900928792568</v>
+      </c>
+      <c r="G5">
+        <f>'High Recoil Spells'!D4  / 'High Recoil Spells'!E4</f>
+        <v>0.43173232595790612</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6">
+        <f>'High Damage Spells'!D5  / 'High Damage Spells'!E5</f>
+        <v>0.82450426680958078</v>
+      </c>
+      <c r="C6">
+        <f>'High Duration Spells'!D5  / 'High Duration Spells'!E5</f>
+        <v>0.7122225299726983</v>
+      </c>
+      <c r="D6">
+        <f>'High Instance Spells'!D5  / 'High Instance Spells'!E5</f>
+        <v>0.56242969628796402</v>
+      </c>
+      <c r="E6">
+        <f>'AOE Spells'!D5  / 'AOE Spells'!E5</f>
+        <v>0.53083252233920197</v>
+      </c>
+      <c r="F6">
+        <f>'High Knockback Spells'!D5  / 'High Knockback Spells'!E5</f>
+        <v>0.82884376295068374</v>
+      </c>
+      <c r="G6">
+        <f>'High Recoil Spells'!D5  / 'High Recoil Spells'!E5</f>
+        <v>0.79462544246189415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7">
+        <f>'High Damage Spells'!D6  / 'High Damage Spells'!E6</f>
+        <v>1.6434625407930878</v>
+      </c>
+      <c r="C7">
+        <f>'High Duration Spells'!D6  / 'High Duration Spells'!E6</f>
+        <v>1.802735651350925</v>
+      </c>
+      <c r="D7">
+        <f>'High Instance Spells'!D6  / 'High Instance Spells'!E6</f>
+        <v>1.3727464079802323</v>
+      </c>
+      <c r="E7">
+        <f>'AOE Spells'!D6  / 'AOE Spells'!E6</f>
+        <v>0.75578173023630768</v>
+      </c>
+      <c r="F7">
+        <f>'High Knockback Spells'!D6  / 'High Knockback Spells'!E6</f>
+        <v>0.94406419636535277</v>
+      </c>
+      <c r="G7">
+        <f>'High Recoil Spells'!D6  / 'High Recoil Spells'!E6</f>
+        <v>0.82280824453861034</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8">
+        <f>'High Damage Spells'!D7  / 'High Damage Spells'!E7</f>
+        <v>2.3326940023845317</v>
+      </c>
+      <c r="C8">
+        <f>'High Duration Spells'!D7  / 'High Duration Spells'!E7</f>
+        <v>1.7413801681675707</v>
+      </c>
+      <c r="D8">
+        <f>'High Instance Spells'!D7  / 'High Instance Spells'!E7</f>
+        <v>2.5257627803596687</v>
+      </c>
+      <c r="E8">
+        <f>'AOE Spells'!D7  / 'AOE Spells'!E7</f>
+        <v>1.6687061964623426</v>
+      </c>
+      <c r="F8">
+        <f>'High Knockback Spells'!D7  / 'High Knockback Spells'!E7</f>
+        <v>1.5633142261594581</v>
+      </c>
+      <c r="G8">
+        <f>'High Recoil Spells'!D7  / 'High Recoil Spells'!E7</f>
+        <v>0.45417385775274777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <f>'High Damage Spells'!D8  / 'High Damage Spells'!E8</f>
+        <v>0.51582286642766872</v>
+      </c>
+      <c r="C9">
+        <f>'High Duration Spells'!D8  / 'High Duration Spells'!E8</f>
+        <v>0.41257189065194616</v>
+      </c>
+      <c r="D9">
+        <f>'High Instance Spells'!D8  / 'High Instance Spells'!E8</f>
+        <v>0.50266411983512616</v>
+      </c>
+      <c r="E9">
+        <f>'AOE Spells'!D8  / 'AOE Spells'!E8</f>
+        <v>0.83024298444678135</v>
+      </c>
+      <c r="F9">
+        <f>'High Knockback Spells'!D8  / 'High Knockback Spells'!E8</f>
+        <v>0.51853772361939332</v>
+      </c>
+      <c r="G9">
+        <f>'High Recoil Spells'!D8  / 'High Recoil Spells'!E8</f>
+        <v>0.75322758018107594</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10">
+        <f>'High Damage Spells'!D9  / 'High Damage Spells'!E9</f>
+        <v>1.9530223020123643</v>
+      </c>
+      <c r="C10">
+        <f>'High Duration Spells'!D9  / 'High Duration Spells'!E9</f>
+        <v>1.2256403971074885</v>
+      </c>
+      <c r="D10">
+        <f>'High Instance Spells'!D9  / 'High Instance Spells'!E9</f>
+        <v>1.4640002342400376</v>
+      </c>
+      <c r="E10">
+        <f>'AOE Spells'!D9  / 'AOE Spells'!E9</f>
+        <v>1.2090339013105929</v>
+      </c>
+      <c r="F10">
+        <f>'High Knockback Spells'!D9  / 'High Knockback Spells'!E9</f>
+        <v>1.0571622744091216</v>
+      </c>
+      <c r="G10">
+        <f>'High Recoil Spells'!D9  / 'High Recoil Spells'!E9</f>
+        <v>1.0530056730680637</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11">
+        <f>'High Damage Spells'!D10  / 'High Damage Spells'!E10</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>'High Duration Spells'!D10  / 'High Duration Spells'!E10</f>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>'High Instance Spells'!D10  / 'High Instance Spells'!E10</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>'AOE Spells'!D10  / 'AOE Spells'!E10</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>'High Knockback Spells'!D10  / 'High Knockback Spells'!E10</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f>'High Recoil Spells'!D10  / 'High Recoil Spells'!E10</f>
+        <v>6.1162079510703373</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12">
+        <f>'High Damage Spells'!D11  / 'High Damage Spells'!E11</f>
+        <v>2.0398449717821445</v>
+      </c>
+      <c r="C12">
+        <f>'High Duration Spells'!D11  / 'High Duration Spells'!E11</f>
+        <v>0.65261371794035106</v>
+      </c>
+      <c r="D12">
+        <f>'High Instance Spells'!D11  / 'High Instance Spells'!E11</f>
+        <v>1.3252054068380599</v>
+      </c>
+      <c r="E12">
+        <f>'AOE Spells'!D11  / 'AOE Spells'!E11</f>
+        <v>0.72960747118050495</v>
+      </c>
+      <c r="F12">
+        <f>'High Knockback Spells'!D11  / 'High Knockback Spells'!E11</f>
+        <v>1.367053998632946</v>
+      </c>
+      <c r="G12">
+        <f>'High Recoil Spells'!D11  / 'High Recoil Spells'!E11</f>
+        <v>2.3829381627546766</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13">
+        <f>'High Damage Spells'!D12  / 'High Damage Spells'!E12</f>
+        <v>2.338482324971094</v>
+      </c>
+      <c r="C13">
+        <f>'High Duration Spells'!D12  / 'High Duration Spells'!E12</f>
+        <v>2.4938588725264039</v>
+      </c>
+      <c r="D13">
+        <f>'High Instance Spells'!D12  / 'High Instance Spells'!E12</f>
+        <v>1.2660150908998835</v>
+      </c>
+      <c r="E13">
+        <f>'AOE Spells'!D12  / 'AOE Spells'!E12</f>
+        <v>1.8122508155128667</v>
+      </c>
+      <c r="F13">
+        <f>'High Knockback Spells'!D12  / 'High Knockback Spells'!E12</f>
+        <v>1.0447956118584301</v>
+      </c>
+      <c r="G13">
+        <f>'High Recoil Spells'!D12  / 'High Recoil Spells'!E12</f>
+        <v>1.3659025200901496</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14">
+        <f>'High Damage Spells'!D13  / 'High Damage Spells'!E13</f>
+        <v>1.7379592014077467</v>
+      </c>
+      <c r="C14">
+        <f>'High Duration Spells'!D13  / 'High Duration Spells'!E13</f>
+        <v>1.4595800579661795</v>
+      </c>
+      <c r="D14">
+        <f>'High Instance Spells'!D13  / 'High Instance Spells'!E13</f>
+        <v>3.8106528918621394</v>
+      </c>
+      <c r="E14">
+        <f>'AOE Spells'!D13  / 'AOE Spells'!E13</f>
+        <v>1.6317777052543241</v>
+      </c>
+      <c r="F14">
+        <f>'High Knockback Spells'!D13  / 'High Knockback Spells'!E13</f>
+        <v>0.8735531775496832</v>
+      </c>
+      <c r="G14">
+        <f>'High Recoil Spells'!D13  / 'High Recoil Spells'!E13</f>
+        <v>1.5227073737104573</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15">
+        <f>'High Damage Spells'!D14  / 'High Damage Spells'!E14</f>
+        <v>0.77564475470234628</v>
+      </c>
+      <c r="C15">
+        <f>'High Duration Spells'!D14  / 'High Duration Spells'!E14</f>
+        <v>0.96780197282709846</v>
+      </c>
+      <c r="D15">
+        <f>'High Instance Spells'!D14  / 'High Instance Spells'!E14</f>
+        <v>1.0582010582010581</v>
+      </c>
+      <c r="E15">
+        <f>'AOE Spells'!D14  / 'AOE Spells'!E14</f>
+        <v>0.99875156054931324</v>
+      </c>
+      <c r="F15">
+        <f>'High Knockback Spells'!D14  / 'High Knockback Spells'!E14</f>
+        <v>1.0916179337231968</v>
+      </c>
+      <c r="G15">
+        <f>'High Recoil Spells'!D14  / 'High Recoil Spells'!E14</f>
+        <v>1.2232415902140674</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16">
+        <f>'High Damage Spells'!D15  / 'High Damage Spells'!E15</f>
+        <v>0.62743567041501391</v>
+      </c>
+      <c r="C16">
+        <f>'High Duration Spells'!D15  / 'High Duration Spells'!E15</f>
+        <v>1.3382491686127043</v>
+      </c>
+      <c r="D16">
+        <f>'High Instance Spells'!D15  / 'High Instance Spells'!E15</f>
+        <v>0.81523954455284109</v>
+      </c>
+      <c r="E16">
+        <f>'AOE Spells'!D15  / 'AOE Spells'!E15</f>
+        <v>0.6732596238722901</v>
+      </c>
+      <c r="F16">
+        <f>'High Knockback Spells'!D15  / 'High Knockback Spells'!E15</f>
+        <v>0.8409839512229309</v>
+      </c>
+      <c r="G16">
+        <f>'High Recoil Spells'!D15  / 'High Recoil Spells'!E15</f>
+        <v>0.9772902185465252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17">
+        <f>'High Damage Spells'!D16  / 'High Damage Spells'!E16</f>
+        <v>0.27127471990885171</v>
+      </c>
+      <c r="C17">
+        <f>'High Duration Spells'!D16  / 'High Duration Spells'!E16</f>
+        <v>1.3018460176530322</v>
+      </c>
+      <c r="D17">
+        <f>'High Instance Spells'!D16  / 'High Instance Spells'!E16</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>'AOE Spells'!D16  / 'AOE Spells'!E16</f>
+        <v>2.0376084298771615</v>
+      </c>
+      <c r="F17">
+        <f>'High Knockback Spells'!D16  / 'High Knockback Spells'!E16</f>
+        <v>0.54540496318516496</v>
+      </c>
+      <c r="G17">
+        <f>'High Recoil Spells'!D16  / 'High Recoil Spells'!E16</f>
+        <v>0.47535294956505209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18">
+        <f>'High Damage Spells'!D17  / 'High Damage Spells'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f>'High Duration Spells'!D17  / 'High Duration Spells'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>'High Instance Spells'!D17  / 'High Instance Spells'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>'AOE Spells'!D17  / 'AOE Spells'!E17</f>
+        <v>5.617977528089888</v>
+      </c>
+      <c r="F18">
+        <f>'High Knockback Spells'!D17  / 'High Knockback Spells'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>'High Recoil Spells'!D17  / 'High Recoil Spells'!E17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19">
+        <f>'High Damage Spells'!D18  / 'High Damage Spells'!E18</f>
+        <v>1.3110856663374384</v>
+      </c>
+      <c r="C19">
+        <f>'High Duration Spells'!D18  / 'High Duration Spells'!E18</f>
+        <v>0.83891913658442463</v>
+      </c>
+      <c r="D19">
+        <f>'High Instance Spells'!D18  / 'High Instance Spells'!E18</f>
+        <v>1.0221116827365335</v>
+      </c>
+      <c r="E19">
+        <f>'AOE Spells'!D18  / 'AOE Spells'!E18</f>
+        <v>1.1254712911031493</v>
+      </c>
+      <c r="F19">
+        <f>'High Knockback Spells'!D18  / 'High Knockback Spells'!E18</f>
+        <v>1.7573148229505313</v>
+      </c>
+      <c r="G19">
+        <f>'High Recoil Spells'!D18  / 'High Recoil Spells'!E18</f>
+        <v>1.5316046622045918</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20">
+        <f>'High Damage Spells'!D19  / 'High Damage Spells'!E19</f>
+        <v>0.66168746846645654</v>
+      </c>
+      <c r="C20">
+        <f>'High Duration Spells'!D19  / 'High Duration Spells'!E19</f>
+        <v>0.95263045083236075</v>
+      </c>
+      <c r="D20">
+        <f>'High Instance Spells'!D19  / 'High Instance Spells'!E19</f>
+        <v>2.2568269013766642</v>
+      </c>
+      <c r="E20">
+        <f>'AOE Spells'!D19  / 'AOE Spells'!E19</f>
+        <v>1.508777535190017</v>
+      </c>
+      <c r="F20">
+        <f>'High Knockback Spells'!D19  / 'High Knockback Spells'!E19</f>
+        <v>1.1640475596574373</v>
+      </c>
+      <c r="G20">
+        <f>'High Recoil Spells'!D19  / 'High Recoil Spells'!E19</f>
+        <v>1.1594707016247083</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21">
+        <f>'High Damage Spells'!D20  / 'High Damage Spells'!E20</f>
+        <v>0.75124533361071621</v>
+      </c>
+      <c r="C21">
+        <f>'High Duration Spells'!D20  / 'High Duration Spells'!E20</f>
+        <v>0.83197444174514945</v>
+      </c>
+      <c r="D21">
+        <f>'High Instance Spells'!D20  / 'High Instance Spells'!E20</f>
+        <v>0.6757669955399378</v>
+      </c>
+      <c r="E21">
+        <f>'AOE Spells'!D20  / 'AOE Spells'!E20</f>
+        <v>0.68209440186521808</v>
+      </c>
+      <c r="F21">
+        <f>'High Knockback Spells'!D20  / 'High Knockback Spells'!E20</f>
+        <v>0.69710700592540953</v>
+      </c>
+      <c r="G21">
+        <f>'High Recoil Spells'!D20  / 'High Recoil Spells'!E20</f>
+        <v>1.1138789314863196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22">
+        <f>'High Damage Spells'!D21  / 'High Damage Spells'!E21</f>
+        <v>0.37939145610440855</v>
+      </c>
+      <c r="C22">
+        <f>'High Duration Spells'!D21  / 'High Duration Spells'!E21</f>
+        <v>0.54620930740659823</v>
+      </c>
+      <c r="D22">
+        <f>'High Instance Spells'!D21  / 'High Instance Spells'!E21</f>
+        <v>1.4788524105294294</v>
+      </c>
+      <c r="E22">
+        <f>'AOE Spells'!D21  / 'AOE Spells'!E21</f>
+        <v>1.0177495521901969</v>
+      </c>
+      <c r="F22">
+        <f>'High Knockback Spells'!D21  / 'High Knockback Spells'!E21</f>
+        <v>2.2883295194508011</v>
+      </c>
+      <c r="G22">
+        <f>'High Recoil Spells'!D21  / 'High Recoil Spells'!E21</f>
+        <v>0.99720781810929415</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23">
+        <f>'High Damage Spells'!D22  / 'High Damage Spells'!E22</f>
+        <v>0.53424511165722832</v>
+      </c>
+      <c r="C23">
+        <f>'High Duration Spells'!D22  / 'High Duration Spells'!E22</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>'High Instance Spells'!D22  / 'High Instance Spells'!E22</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>'AOE Spells'!D22  / 'AOE Spells'!E22</f>
+        <v>1.1465260261407935</v>
+      </c>
+      <c r="F23">
+        <f>'High Knockback Spells'!D22  / 'High Knockback Spells'!E22</f>
+        <v>1.0741138560687433</v>
+      </c>
+      <c r="G23">
+        <f>'High Recoil Spells'!D22  / 'High Recoil Spells'!E22</f>
+        <v>0.93615427822505159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24">
+        <f>'High Damage Spells'!D23  / 'High Damage Spells'!E23</f>
+        <v>1.1092377318306859</v>
+      </c>
+      <c r="C24">
+        <f>'High Duration Spells'!D23  / 'High Duration Spells'!E23</f>
+        <v>0.42585810407972063</v>
+      </c>
+      <c r="D24">
+        <f>'High Instance Spells'!D23  / 'High Instance Spells'!E23</f>
+        <v>0.43237634036665518</v>
+      </c>
+      <c r="E24">
+        <f>'AOE Spells'!D23  / 'AOE Spells'!E23</f>
+        <v>0.47609979051609225</v>
+      </c>
+      <c r="F24">
+        <f>'High Knockback Spells'!D23  / 'High Knockback Spells'!E23</f>
+        <v>1.3380909901873328</v>
+      </c>
+      <c r="G24">
+        <f>'High Recoil Spells'!D23  / 'High Recoil Spells'!E23</f>
+        <v>0.77748406157673777</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25">
+        <f>'High Damage Spells'!D24  / 'High Damage Spells'!E24</f>
+        <v>6.9808027923211169</v>
+      </c>
+      <c r="C25">
+        <f>'High Duration Spells'!D24  / 'High Duration Spells'!E24</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>'High Instance Spells'!D24  / 'High Instance Spells'!E24</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f>'AOE Spells'!D24  / 'AOE Spells'!E24</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f>'High Knockback Spells'!D24  / 'High Knockback Spells'!E24</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>'High Recoil Spells'!D24  / 'High Recoil Spells'!E24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26">
+        <f>'High Damage Spells'!D25  / 'High Damage Spells'!E25</f>
+        <v>0.26576660376857042</v>
+      </c>
+      <c r="C26">
+        <f>'High Duration Spells'!D25  / 'High Duration Spells'!E25</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>'High Instance Spells'!D25  / 'High Instance Spells'!E25</f>
+        <v>0.51797368693670365</v>
+      </c>
+      <c r="E26">
+        <f>'AOE Spells'!D25  / 'AOE Spells'!E25</f>
+        <v>0.57035304853704449</v>
+      </c>
+      <c r="F26">
+        <f>'High Knockback Spells'!D25  / 'High Knockback Spells'!E25</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>'High Recoil Spells'!D25  / 'High Recoil Spells'!E25</f>
+        <v>0.46570111302566014</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27">
+        <f>'High Damage Spells'!D26  / 'High Damage Spells'!E26</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>'High Duration Spells'!D26  / 'High Duration Spells'!E26</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>'High Instance Spells'!D26  / 'High Instance Spells'!E26</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>'AOE Spells'!D26  / 'AOE Spells'!E26</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>'High Knockback Spells'!D26  / 'High Knockback Spells'!E26</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>'High Recoil Spells'!D26  / 'High Recoil Spells'!E26</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>